<commit_message>
DataType import export nem romlik el
</commit_message>
<xml_diff>
--- a/papyrus.teszt/excel/prop2.xlsx
+++ b/papyrus.teszt/excel/prop2.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="85">
   <si>
     <t>XmiId</t>
   </si>
@@ -207,6 +207,12 @@
     <t>Paraméter név</t>
   </si>
   <si>
+    <t>_Gql2AFYYEeyzWIy-BpzvfQ</t>
+  </si>
+  <si>
+    <t>parentProp1</t>
+  </si>
+  <si>
     <t>_dex_gFYYEeyzWIy-BpzvfQ</t>
   </si>
   <si>
@@ -219,9 +225,6 @@
     <t>String</t>
   </si>
   <si>
-    <t>returnParam</t>
-  </si>
-  <si>
     <t>param1</t>
   </si>
   <si>
@@ -237,12 +240,6 @@
     <t>parentOperation2</t>
   </si>
   <si>
-    <t>_Gql2AFYYEeyzWIy-BpzvfQ</t>
-  </si>
-  <si>
-    <t>parentProp1</t>
-  </si>
-  <si>
     <t>Static</t>
   </si>
   <si>
@@ -271,9 +268,6 @@
   </si>
   <si>
     <t>igen</t>
-  </si>
-  <si>
-    <t>returnttttt</t>
   </si>
   <si>
     <t>aaaaaa</t>
@@ -455,7 +449,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -463,7 +457,7 @@
   <cols>
     <col min="1" max="1" width="13.5703125" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="27.77734375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="20.5390625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="15.671875" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="11.0546875" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="8.36328125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="8.76171875" customWidth="true" bestFit="true"/>
@@ -490,7 +484,7 @@
         <v>46</v>
       </c>
       <c r="F1" t="s" s="14">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G1" t="s" s="14">
         <v>28</v>
@@ -502,10 +496,10 @@
         <v>23</v>
       </c>
       <c r="B2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" t="s">
         <v>74</v>
-      </c>
-      <c r="C2" t="s">
-        <v>75</v>
       </c>
       <c r="D2" t="s">
         <v>30</v>
@@ -526,10 +520,10 @@
         <v>23</v>
       </c>
       <c r="B3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" t="s">
         <v>76</v>
-      </c>
-      <c r="C3" t="s">
-        <v>77</v>
       </c>
       <c r="D3" t="s">
         <v>30</v>
@@ -550,10 +544,10 @@
         <v>23</v>
       </c>
       <c r="B4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" t="s">
         <v>78</v>
-      </c>
-      <c r="C4" t="s">
-        <v>79</v>
       </c>
       <c r="D4" t="s">
         <v>30</v>
@@ -583,7 +577,7 @@
         <v>26</v>
       </c>
       <c r="E6" t="s" s="15">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F6" t="s" s="15">
         <v>57</v>
@@ -601,61 +595,6 @@
         <v>28</v>
       </c>
       <c r="K6" s="15"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" t="s">
-        <v>80</v>
-      </c>
-      <c r="C7" t="s">
-        <v>81</v>
-      </c>
-      <c r="D7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" t="s">
-        <v>82</v>
-      </c>
-      <c r="F7" t="s">
-        <v>82</v>
-      </c>
-      <c r="G7" t="s">
-        <v>64</v>
-      </c>
-      <c r="H7" t="s">
-        <v>64</v>
-      </c>
-      <c r="I7" t="s">
-        <v>83</v>
-      </c>
-      <c r="J7" t="s">
-        <v>23</v>
-      </c>
-      <c r="K7"/>
-    </row>
-    <row r="8">
-      <c r="F8" t="s">
-        <v>49</v>
-      </c>
-      <c r="G8" t="s">
-        <v>84</v>
-      </c>
-      <c r="H8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="F9" t="s">
-        <v>85</v>
-      </c>
-      <c r="G9" t="s">
-        <v>86</v>
-      </c>
-      <c r="H9" t="s">
-        <v>23</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -699,7 +638,7 @@
         <v>46</v>
       </c>
       <c r="F1" t="s" s="16">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G1" t="s" s="16">
         <v>28</v>
@@ -711,10 +650,10 @@
         <v>23</v>
       </c>
       <c r="B2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" t="s">
         <v>78</v>
-      </c>
-      <c r="C2" t="s">
-        <v>79</v>
       </c>
       <c r="D2" t="s">
         <v>30</v>
@@ -744,7 +683,7 @@
         <v>26</v>
       </c>
       <c r="E4" t="s" s="17">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F4" t="s" s="17">
         <v>57</v>
@@ -768,53 +707,53 @@
         <v>23</v>
       </c>
       <c r="B5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" t="s">
         <v>80</v>
-      </c>
-      <c r="C5" t="s">
-        <v>81</v>
       </c>
       <c r="D5" t="s">
         <v>30</v>
       </c>
       <c r="E5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F5" t="s">
+        <v>81</v>
+      </c>
+      <c r="G5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I5" t="s">
         <v>82</v>
       </c>
-      <c r="F5" t="s">
+      <c r="J5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5"/>
+    </row>
+    <row r="6">
+      <c r="H6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I6" t="s">
         <v>82</v>
       </c>
-      <c r="G5" t="s">
-        <v>64</v>
-      </c>
-      <c r="H5" t="s">
-        <v>64</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="J6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="H7" t="s">
         <v>83</v>
       </c>
-      <c r="J5" t="s">
-        <v>23</v>
-      </c>
-      <c r="K5"/>
-    </row>
-    <row r="6">
-      <c r="F6" t="s">
-        <v>49</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="I7" t="s">
         <v>84</v>
       </c>
-      <c r="H6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="F7" t="s">
-        <v>85</v>
-      </c>
-      <c r="G7" t="s">
-        <v>86</v>
-      </c>
-      <c r="H7" t="s">
+      <c r="J7" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1239,7 +1178,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1247,7 +1186,7 @@
   <cols>
     <col min="1" max="1" width="13.5703125" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="27.58203125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="17.203125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="11.59765625" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="11.0546875" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="8.76171875" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="17.10546875" customWidth="true" bestFit="true"/>
@@ -1357,99 +1296,6 @@
         <v>28</v>
       </c>
       <c r="J6" s="7"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7" t="s">
-        <v>63</v>
-      </c>
-      <c r="E7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" t="s">
-        <v>64</v>
-      </c>
-      <c r="G7" t="s">
-        <v>64</v>
-      </c>
-      <c r="H7" t="s">
-        <v>65</v>
-      </c>
-      <c r="I7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J7"/>
-    </row>
-    <row r="8">
-      <c r="G8" t="s">
-        <v>64</v>
-      </c>
-      <c r="H8" t="s">
-        <v>66</v>
-      </c>
-      <c r="I8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="G9" t="s">
-        <v>49</v>
-      </c>
-      <c r="H9" t="s">
-        <v>67</v>
-      </c>
-      <c r="I9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="G10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H10" t="s">
-        <v>68</v>
-      </c>
-      <c r="I10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" t="s">
-        <v>69</v>
-      </c>
-      <c r="C11" t="s">
-        <v>70</v>
-      </c>
-      <c r="D11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" t="s">
-        <v>40</v>
-      </c>
-      <c r="F11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G11" t="s">
-        <v>23</v>
-      </c>
-      <c r="H11" t="s">
-        <v>23</v>
-      </c>
-      <c r="I11" t="s">
-        <v>23</v>
-      </c>
-      <c r="J11"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -1642,10 +1488,10 @@
         <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="D2" t="s">
         <v>55</v>
@@ -1708,25 +1554,25 @@
         <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C6" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E6" t="s">
         <v>40</v>
       </c>
       <c r="F6" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G6" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="I6" t="s">
         <v>23</v>
@@ -1735,10 +1581,10 @@
     </row>
     <row r="7">
       <c r="G7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I7" t="s">
         <v>23</v>
@@ -1749,7 +1595,7 @@
         <v>49</v>
       </c>
       <c r="H8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I8" t="s">
         <v>23</v>
@@ -1757,10 +1603,10 @@
     </row>
     <row r="9">
       <c r="G9" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I9" t="s">
         <v>23</v>
@@ -1771,10 +1617,10 @@
         <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C10" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D10" t="s">
         <v>30</v>

</xml_diff>